<commit_message>
Revert "Merge branch 'master' of https://github.com/Dopa99/Unix-TermProject"
This reverts commit 7c590aeac7f0a9f7051adb883092ecdec7da39fd, reversing
changes made to 45dd50bc6bd28ed303e70665e1c2df353d9f1716.
</commit_message>
<xml_diff>
--- a/DataPack규칙.xlsx
+++ b/DataPack규칙.xlsx
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>